<commit_message>
3d frame examples added: 3d-2side-static-elastic, 3d-simple-beam-static-elastic, 3d-2side-dynamic-elastic, 3d-simple-beam-dynamic-elastic
</commit_message>
<xml_diff>
--- a/comparison/1story-dynamic-elastic.xlsx
+++ b/comparison/1story-dynamic-elastic.xlsx
@@ -143,7 +143,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -894,11 +893,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="375973184"/>
-        <c:axId val="375972008"/>
+        <c:axId val="312284920"/>
+        <c:axId val="312285312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="375973184"/>
+        <c:axId val="312284920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -955,12 +954,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375972008"/>
+        <c:crossAx val="312285312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="375972008"/>
+        <c:axId val="312285312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1017,7 +1016,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375973184"/>
+        <c:crossAx val="312284920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1031,7 +1030,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1867,11 +1865,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="312704080"/>
-        <c:axId val="312706040"/>
+        <c:axId val="312287664"/>
+        <c:axId val="312286096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="312704080"/>
+        <c:axId val="312287664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1928,12 +1926,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312706040"/>
+        <c:crossAx val="312286096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="312706040"/>
+        <c:axId val="312286096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1990,7 +1988,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312704080"/>
+        <c:crossAx val="312287664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4140,7 +4138,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>